<commit_message>
CMS Connectathon - ExampleScenarios, TestScripts, Extensions
</commit_message>
<xml_diff>
--- a/output/CodeSystem-AcceptingPatientsCS.xlsx
+++ b/output/CodeSystem-AcceptingPatientsCS.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.4</t>
+    <t>0.1.6</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-06-03T13:24:40-05:00</t>
+    <t>2022-06-15T12:17:27-04:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>